<commit_message>
Invoice Genration UI made
</commit_message>
<xml_diff>
--- a/output/invoice.xlsx
+++ b/output/invoice.xlsx
@@ -27,13 +27,13 @@
     <t>Email: sunny.printers@gmail.com| Ph: 9811269375 9999662547</t>
   </si>
   <si>
-    <t>Date: 2026-01-04</t>
+    <t>Date: 2026-01-05</t>
   </si>
   <si>
     <t>Client: Tarun Shah</t>
   </si>
   <si>
-    <t>Performa No: INV-1767520377318</t>
+    <t>Performa No: INV-1767593299989</t>
   </si>
   <si>
     <t>#</t>

</xml_diff>

<commit_message>
Card 1 and 2 Final functioning on invoice Genration
</commit_message>
<xml_diff>
--- a/output/invoice.xlsx
+++ b/output/invoice.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Invoice" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Invoice!$A$1:$D$228</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Invoice!$A$1:$D$209</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="56">
   <si>
     <t>SUNNY PRINTERS</t>
   </si>
@@ -27,13 +27,13 @@
     <t>Email: sunny.printers@gmail.com | Ph: 9811269375 9999662547</t>
   </si>
   <si>
-    <t>Date: 2026-01-10</t>
-  </si>
-  <si>
-    <t>Client: Tarun Shah</t>
-  </si>
-  <si>
-    <t>Performa No: INV-1768061550069</t>
+    <t>Date: 2026-01-14</t>
+  </si>
+  <si>
+    <t>Client: Royal Graphics (Tarun Shah)</t>
+  </si>
+  <si>
+    <t>Performa No: INV-1768388226087</t>
   </si>
   <si>
     <t>#</t>
@@ -48,55 +48,22 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>(JOB-1001) - Visiting Card Printing</t>
-  </si>
-  <si>
-    <t>Visiting card printing (500 qty)</t>
-  </si>
-  <si>
-    <t>300 GSM art card</t>
-  </si>
-  <si>
-    <t>Matt lamination</t>
-  </si>
-  <si>
-    <t>(JOB-1002) - Letterhead Printing</t>
-  </si>
-  <si>
-    <t>Letterhead printing (1000 qty)</t>
-  </si>
-  <si>
-    <t>Executive bond paper</t>
+    <t>(RG-TS-301) - Visiting Card Printing</t>
+  </si>
+  <si>
+    <t>Printing charges</t>
+  </si>
+  <si>
+    <t>Paper material</t>
+  </si>
+  <si>
+    <t>Gloss/Matt lamination</t>
+  </si>
+  <si>
+    <t>(RG-TS-302) - Pamphlet Printing</t>
   </si>
   <si>
     <t>CTP plate charges</t>
-  </si>
-  <si>
-    <t>Gloss/Matt lamination</t>
-  </si>
-  <si>
-    <t>(JOB-1003) - Brochure Printing</t>
-  </si>
-  <si>
-    <t>Brochure printing</t>
-  </si>
-  <si>
-    <t>170 GSM art paper</t>
-  </si>
-  <si>
-    <t>Center fold</t>
-  </si>
-  <si>
-    <t>(RG-TS-301) - Visiting Card Printing</t>
-  </si>
-  <si>
-    <t>Printing charges</t>
-  </si>
-  <si>
-    <t>Paper material</t>
-  </si>
-  <si>
-    <t>(RG-TS-302) - Pamphlet Printing</t>
   </si>
   <si>
     <t>(RG-TS-303) - Poster Printing</t>
@@ -758,7 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D228"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="true"/>
+  </sheetPr>
+  <dimension ref="A1:D209"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -845,7 +815,7 @@
         <v>1.0</v>
       </c>
       <c r="B10" t="n" s="17">
-        <v>45662.0</v>
+        <v>46026.0</v>
       </c>
       <c r="C10" t="s" s="19">
         <v>10</v>
@@ -858,635 +828,633 @@
         <v>11</v>
       </c>
       <c r="D11" t="n" s="20">
-        <v>1200.0</v>
+        <v>2500.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="27"/>
       <c r="C12" t="s" s="19">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D12" t="n" s="20">
-        <v>1200.0</v>
+        <v>2400.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="27"/>
       <c r="C13" t="s" s="19">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" t="n" s="20">
-        <v>600.0</v>
+        <v>1200.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="27"/>
-      <c r="C14" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D14" t="n" s="20">
-        <v>300.0</v>
-      </c>
+      <c r="D14" s="31"/>
     </row>
     <row r="15">
-      <c r="A15" s="27"/>
-      <c r="D15" s="31"/>
+      <c r="A15" t="n" s="16">
+        <v>2.0</v>
+      </c>
+      <c r="B15" t="n" s="17">
+        <v>46026.0</v>
+      </c>
+      <c r="C15" t="s" s="19">
+        <v>14</v>
+      </c>
+      <c r="D15" s="16"/>
     </row>
     <row r="16">
-      <c r="A16" t="n" s="16">
-        <v>2.0</v>
-      </c>
-      <c r="B16" t="n" s="17">
-        <v>45665.0</v>
-      </c>
+      <c r="A16" s="27"/>
       <c r="C16" t="s" s="19">
-        <v>14</v>
-      </c>
-      <c r="D16" s="16"/>
+        <v>11</v>
+      </c>
+      <c r="D16" t="n" s="20">
+        <v>2900.0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="27"/>
       <c r="C17" t="s" s="19">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D17" t="n" s="20">
-        <v>1500.0</v>
+        <v>2700.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="27"/>
       <c r="C18" t="s" s="19">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D18" t="n" s="20">
-        <v>600.0</v>
+        <v>1600.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="27"/>
-      <c r="C19" t="s" s="19">
+      <c r="D19" s="31"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="n" s="16">
+        <v>3.0</v>
+      </c>
+      <c r="B20" t="n" s="17">
+        <v>46026.0</v>
+      </c>
+      <c r="C20" t="s" s="19">
         <v>16</v>
       </c>
-      <c r="D19" t="n" s="20">
-        <v>800.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="27"/>
-      <c r="C20" t="s" s="19">
-        <v>17</v>
-      </c>
-      <c r="D20" t="n" s="20">
-        <v>1600.0</v>
-      </c>
+      <c r="D20" s="16"/>
     </row>
     <row r="21">
       <c r="A21" s="27"/>
       <c r="C21" t="s" s="19">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D21" t="n" s="20">
-        <v>1200.0</v>
+        <v>3300.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="27"/>
-      <c r="D22" s="31"/>
+      <c r="C22" t="s" s="19">
+        <v>12</v>
+      </c>
+      <c r="D22" t="n" s="20">
+        <v>1800.0</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" t="n" s="16">
-        <v>3.0</v>
-      </c>
-      <c r="B23" t="n" s="17">
-        <v>45667.0</v>
-      </c>
+      <c r="A23" s="27"/>
       <c r="C23" t="s" s="19">
-        <v>19</v>
-      </c>
-      <c r="D23" s="16"/>
+        <v>13</v>
+      </c>
+      <c r="D23" t="n" s="20">
+        <v>1200.0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="27"/>
-      <c r="C24" t="s" s="19">
-        <v>20</v>
-      </c>
-      <c r="D24" t="n" s="20">
-        <v>2500.0</v>
-      </c>
+      <c r="D24" s="31"/>
     </row>
     <row r="25">
-      <c r="A25" s="27"/>
+      <c r="A25" t="n" s="16">
+        <v>4.0</v>
+      </c>
+      <c r="B25" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C25" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="D25" t="n" s="20">
-        <v>1200.0</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D25" s="16"/>
     </row>
     <row r="26">
       <c r="A26" s="27"/>
       <c r="C26" t="s" s="19">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D26" t="n" s="20">
-        <v>300.0</v>
+        <v>3700.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="27"/>
       <c r="C27" t="s" s="19">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D27" t="n" s="20">
-        <v>400.0</v>
+        <v>2100.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="27"/>
-      <c r="D28" s="31"/>
+      <c r="C28" t="s" s="19">
+        <v>18</v>
+      </c>
+      <c r="D28" t="n" s="20">
+        <v>1400.0</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" t="n" s="16">
-        <v>4.0</v>
-      </c>
-      <c r="B29" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C29" t="s" s="19">
-        <v>23</v>
-      </c>
-      <c r="D29" s="16"/>
+      <c r="A29" s="27"/>
+      <c r="D29" s="31"/>
     </row>
     <row r="30">
-      <c r="A30" s="27"/>
+      <c r="A30" t="n" s="16">
+        <v>5.0</v>
+      </c>
+      <c r="B30" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C30" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D30" t="n" s="20">
-        <v>2500.0</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D30" s="16"/>
     </row>
     <row r="31">
       <c r="A31" s="27"/>
       <c r="C31" t="s" s="19">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D31" t="n" s="20">
-        <v>2400.0</v>
+        <v>4100.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="27"/>
       <c r="C32" t="s" s="19">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D32" t="n" s="20">
-        <v>1200.0</v>
+        <v>2400.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="27"/>
-      <c r="D33" s="31"/>
+      <c r="C33" t="s" s="19">
+        <v>15</v>
+      </c>
+      <c r="D33" t="n" s="20">
+        <v>1600.0</v>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" t="n" s="16">
-        <v>5.0</v>
-      </c>
-      <c r="B34" t="n" s="17">
-        <v>46026.0</v>
-      </c>
+      <c r="A34" s="27"/>
       <c r="C34" t="s" s="19">
-        <v>26</v>
-      </c>
-      <c r="D34" s="16"/>
+        <v>13</v>
+      </c>
+      <c r="D34" t="n" s="20">
+        <v>1200.0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="27"/>
-      <c r="C35" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D35" t="n" s="20">
-        <v>2900.0</v>
-      </c>
+      <c r="D35" s="31"/>
     </row>
     <row r="36">
-      <c r="A36" s="27"/>
+      <c r="A36" t="n" s="16">
+        <v>6.0</v>
+      </c>
+      <c r="B36" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C36" t="s" s="19">
-        <v>25</v>
-      </c>
-      <c r="D36" t="n" s="20">
-        <v>2700.0</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D36" s="16"/>
     </row>
     <row r="37">
       <c r="A37" s="27"/>
       <c r="C37" t="s" s="19">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D37" t="n" s="20">
-        <v>1600.0</v>
+        <v>2500.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="27"/>
-      <c r="D38" s="31"/>
+      <c r="C38" t="s" s="19">
+        <v>12</v>
+      </c>
+      <c r="D38" t="n" s="20">
+        <v>2700.0</v>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" t="n" s="16">
-        <v>6.0</v>
-      </c>
-      <c r="B39" t="n" s="17">
-        <v>46026.0</v>
-      </c>
+      <c r="A39" s="27"/>
       <c r="C39" t="s" s="19">
-        <v>27</v>
-      </c>
-      <c r="D39" s="16"/>
+        <v>18</v>
+      </c>
+      <c r="D39" t="n" s="20">
+        <v>1400.0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="27"/>
-      <c r="C40" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D40" t="n" s="20">
-        <v>3300.0</v>
-      </c>
+      <c r="D40" s="31"/>
     </row>
     <row r="41">
-      <c r="A41" s="27"/>
+      <c r="A41" t="n" s="16">
+        <v>7.0</v>
+      </c>
+      <c r="B41" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C41" t="s" s="19">
-        <v>25</v>
-      </c>
-      <c r="D41" t="n" s="20">
-        <v>1800.0</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D41" s="16"/>
     </row>
     <row r="42">
       <c r="A42" s="27"/>
       <c r="C42" t="s" s="19">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D42" t="n" s="20">
-        <v>1200.0</v>
+        <v>2900.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="27"/>
-      <c r="D43" s="31"/>
+      <c r="C43" t="s" s="19">
+        <v>12</v>
+      </c>
+      <c r="D43" t="n" s="20">
+        <v>1800.0</v>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" t="n" s="16">
-        <v>7.0</v>
-      </c>
-      <c r="B44" t="n" s="17">
-        <v>46026.0</v>
-      </c>
+      <c r="A44" s="27"/>
       <c r="C44" t="s" s="19">
-        <v>28</v>
-      </c>
-      <c r="D44" s="16"/>
+        <v>13</v>
+      </c>
+      <c r="D44" t="n" s="20">
+        <v>1200.0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="27"/>
-      <c r="C45" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D45" t="n" s="20">
-        <v>3700.0</v>
-      </c>
+      <c r="D45" s="31"/>
     </row>
     <row r="46">
-      <c r="A46" s="27"/>
+      <c r="A46" t="n" s="16">
+        <v>8.0</v>
+      </c>
+      <c r="B46" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C46" t="s" s="19">
-        <v>25</v>
-      </c>
-      <c r="D46" t="n" s="20">
-        <v>2100.0</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D46" s="16"/>
     </row>
     <row r="47">
       <c r="A47" s="27"/>
       <c r="C47" t="s" s="19">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="D47" t="n" s="20">
-        <v>1400.0</v>
+        <v>3300.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="27"/>
-      <c r="D48" s="31"/>
+      <c r="C48" t="s" s="19">
+        <v>12</v>
+      </c>
+      <c r="D48" t="n" s="20">
+        <v>2100.0</v>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" t="n" s="16">
-        <v>8.0</v>
-      </c>
-      <c r="B49" t="n" s="17">
-        <v>46026.0</v>
-      </c>
+      <c r="A49" s="27"/>
       <c r="C49" t="s" s="19">
-        <v>30</v>
-      </c>
-      <c r="D49" s="16"/>
+        <v>15</v>
+      </c>
+      <c r="D49" t="n" s="20">
+        <v>1600.0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="27"/>
-      <c r="C50" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D50" t="n" s="20">
-        <v>4100.0</v>
-      </c>
+      <c r="D50" s="31"/>
     </row>
     <row r="51">
-      <c r="A51" s="27"/>
+      <c r="A51" t="n" s="16">
+        <v>9.0</v>
+      </c>
+      <c r="B51" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C51" t="s" s="19">
-        <v>25</v>
-      </c>
-      <c r="D51" t="n" s="20">
-        <v>2400.0</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D51" s="16"/>
     </row>
     <row r="52">
       <c r="A52" s="27"/>
       <c r="C52" t="s" s="19">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D52" t="n" s="20">
-        <v>1600.0</v>
+        <v>3700.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="27"/>
       <c r="C53" t="s" s="19">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D53" t="n" s="20">
-        <v>1200.0</v>
+        <v>2400.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="27"/>
-      <c r="D54" s="31"/>
+      <c r="C54" t="s" s="19">
+        <v>13</v>
+      </c>
+      <c r="D54" t="n" s="20">
+        <v>1200.0</v>
+      </c>
     </row>
     <row r="55">
-      <c r="A55" t="n" s="16">
-        <v>9.0</v>
-      </c>
-      <c r="B55" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C55" t="s" s="19">
-        <v>31</v>
-      </c>
-      <c r="D55" s="16"/>
+      <c r="A55" s="27"/>
+      <c r="D55" s="31"/>
     </row>
     <row r="56">
-      <c r="A56" s="27"/>
+      <c r="A56" t="n" s="16">
+        <v>10.0</v>
+      </c>
+      <c r="B56" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C56" t="s" s="19">
         <v>24</v>
       </c>
-      <c r="D56" t="n" s="20">
-        <v>2500.0</v>
-      </c>
+      <c r="D56" s="16"/>
     </row>
     <row r="57">
       <c r="A57" s="27"/>
       <c r="C57" t="s" s="19">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D57" t="n" s="20">
-        <v>2700.0</v>
+        <v>4100.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="27"/>
       <c r="C58" t="s" s="19">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D58" t="n" s="20">
-        <v>1400.0</v>
+        <v>2700.0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="27"/>
-      <c r="D59" s="31"/>
+      <c r="C59" t="s" s="19">
+        <v>18</v>
+      </c>
+      <c r="D59" t="n" s="20">
+        <v>1400.0</v>
+      </c>
     </row>
     <row r="60">
-      <c r="A60" t="n" s="16">
-        <v>10.0</v>
-      </c>
-      <c r="B60" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C60" t="s" s="19">
-        <v>32</v>
-      </c>
-      <c r="D60" s="16"/>
+      <c r="A60" s="27"/>
+      <c r="D60" s="31"/>
     </row>
     <row r="61">
-      <c r="A61" s="27"/>
+      <c r="A61" t="n" s="16">
+        <v>11.0</v>
+      </c>
+      <c r="B61" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C61" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D61" t="n" s="20">
-        <v>2900.0</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D61" s="16"/>
     </row>
     <row r="62">
       <c r="A62" s="27"/>
       <c r="C62" t="s" s="19">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D62" t="n" s="20">
-        <v>1800.0</v>
+        <v>2500.0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="27"/>
       <c r="C63" t="s" s="19">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D63" t="n" s="20">
-        <v>1200.0</v>
+        <v>1800.0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="27"/>
-      <c r="D64" s="31"/>
+      <c r="C64" t="s" s="19">
+        <v>15</v>
+      </c>
+      <c r="D64" t="n" s="20">
+        <v>1600.0</v>
+      </c>
     </row>
     <row r="65">
-      <c r="A65" t="n" s="16">
-        <v>11.0</v>
-      </c>
-      <c r="B65" t="n" s="17">
-        <v>46026.0</v>
-      </c>
+      <c r="A65" s="27"/>
       <c r="C65" t="s" s="19">
-        <v>33</v>
-      </c>
-      <c r="D65" s="16"/>
+        <v>13</v>
+      </c>
+      <c r="D65" t="n" s="20">
+        <v>1200.0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="27"/>
-      <c r="C66" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D66" t="n" s="20">
-        <v>3300.0</v>
-      </c>
+      <c r="D66" s="31"/>
     </row>
     <row r="67">
-      <c r="A67" s="27"/>
+      <c r="A67" t="n" s="16">
+        <v>12.0</v>
+      </c>
+      <c r="B67" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C67" t="s" s="19">
-        <v>25</v>
-      </c>
-      <c r="D67" t="n" s="20">
-        <v>2100.0</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D67" s="16"/>
     </row>
     <row r="68">
       <c r="A68" s="27"/>
       <c r="C68" t="s" s="19">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D68" t="n" s="20">
-        <v>1600.0</v>
+        <v>2900.0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="27"/>
-      <c r="D69" s="31"/>
+      <c r="C69" t="s" s="19">
+        <v>12</v>
+      </c>
+      <c r="D69" t="n" s="20">
+        <v>2100.0</v>
+      </c>
     </row>
     <row r="70">
-      <c r="A70" t="n" s="16">
-        <v>12.0</v>
-      </c>
-      <c r="B70" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C70" t="s" s="19">
-        <v>34</v>
-      </c>
-      <c r="D70" s="16"/>
+      <c r="A70" s="27"/>
+      <c r="D70" s="31"/>
     </row>
     <row r="71">
-      <c r="A71" s="27"/>
+      <c r="A71" t="n" s="16">
+        <v>13.0</v>
+      </c>
+      <c r="B71" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C71" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D71" t="n" s="20">
-        <v>3700.0</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D71" s="16"/>
     </row>
     <row r="72">
       <c r="A72" s="27"/>
       <c r="C72" t="s" s="19">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D72" t="n" s="20">
-        <v>2400.0</v>
+        <v>3300.0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="27"/>
       <c r="C73" t="s" s="19">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D73" t="n" s="20">
-        <v>1200.0</v>
+        <v>2400.0</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="27"/>
-      <c r="D74" s="31"/>
+      <c r="C74" t="s" s="19">
+        <v>13</v>
+      </c>
+      <c r="D74" t="n" s="20">
+        <v>1200.0</v>
+      </c>
     </row>
     <row r="75">
-      <c r="A75" t="n" s="16">
-        <v>13.0</v>
-      </c>
-      <c r="B75" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C75" t="s" s="19">
-        <v>35</v>
-      </c>
-      <c r="D75" s="16"/>
+      <c r="A75" s="27"/>
+      <c r="D75" s="31"/>
     </row>
     <row r="76">
-      <c r="A76" s="27"/>
+      <c r="A76" t="n" s="16">
+        <v>14.0</v>
+      </c>
+      <c r="B76" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C76" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D76" t="n" s="20">
-        <v>4100.0</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D76" s="16"/>
     </row>
     <row r="77">
       <c r="A77" s="27"/>
       <c r="C77" t="s" s="19">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D77" t="n" s="20">
-        <v>2700.0</v>
+        <v>3700.0</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="27"/>
       <c r="C78" t="s" s="19">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D78" t="n" s="20">
-        <v>1400.0</v>
+        <v>2700.0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="27"/>
-      <c r="D79" s="31"/>
+      <c r="C79" t="s" s="19">
+        <v>15</v>
+      </c>
+      <c r="D79" t="n" s="20">
+        <v>1600.0</v>
+      </c>
     </row>
     <row r="80">
-      <c r="A80" t="n" s="16">
-        <v>14.0</v>
-      </c>
-      <c r="B80" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C80" t="s" s="19">
-        <v>36</v>
-      </c>
-      <c r="D80" s="16"/>
+      <c r="A80" s="27"/>
+      <c r="D80" s="31"/>
     </row>
     <row r="81">
-      <c r="A81" s="27"/>
+      <c r="A81" t="n" s="16">
+        <v>15.0</v>
+      </c>
+      <c r="B81" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C81" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D81" t="n" s="20">
-        <v>2500.0</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D81" s="16"/>
     </row>
     <row r="82">
       <c r="A82" s="27"/>
       <c r="C82" t="s" s="19">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D82" t="n" s="20">
-        <v>1800.0</v>
+        <v>4100.0</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="27"/>
       <c r="C83" t="s" s="19">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D83" t="n" s="20">
-        <v>1600.0</v>
+        <v>1800.0</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="27"/>
       <c r="C84" t="s" s="19">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D84" t="n" s="20">
         <v>1200.0</v>
@@ -1498,29 +1466,29 @@
     </row>
     <row r="86">
       <c r="A86" t="n" s="16">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="B86" t="n" s="17">
         <v>46026.0</v>
       </c>
       <c r="C86" t="s" s="19">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D86" s="16"/>
     </row>
     <row r="87">
       <c r="A87" s="27"/>
       <c r="C87" t="s" s="19">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D87" t="n" s="20">
-        <v>2900.0</v>
+        <v>2500.0</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="27"/>
       <c r="C88" t="s" s="19">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D88" t="n" s="20">
         <v>2100.0</v>
@@ -1532,29 +1500,29 @@
     </row>
     <row r="90">
       <c r="A90" t="n" s="16">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
       <c r="B90" t="n" s="17">
         <v>46026.0</v>
       </c>
       <c r="C90" t="s" s="19">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D90" s="16"/>
     </row>
     <row r="91">
       <c r="A91" s="27"/>
       <c r="C91" t="s" s="19">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D91" t="n" s="20">
-        <v>3300.0</v>
+        <v>2900.0</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="27"/>
       <c r="C92" t="s" s="19">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D92" t="n" s="20">
         <v>2400.0</v>
@@ -1563,53 +1531,53 @@
     <row r="93">
       <c r="A93" s="27"/>
       <c r="C93" t="s" s="19">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D93" t="n" s="20">
-        <v>1200.0</v>
+        <v>1600.0</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="27"/>
-      <c r="D94" s="31"/>
+      <c r="C94" t="s" s="19">
+        <v>13</v>
+      </c>
+      <c r="D94" t="n" s="20">
+        <v>1200.0</v>
+      </c>
     </row>
     <row r="95">
-      <c r="A95" t="n" s="16">
-        <v>17.0</v>
-      </c>
-      <c r="B95" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C95" t="s" s="19">
-        <v>39</v>
-      </c>
-      <c r="D95" s="16"/>
+      <c r="A95" s="27"/>
+      <c r="D95" s="31"/>
     </row>
     <row r="96">
-      <c r="A96" s="27"/>
+      <c r="A96" t="n" s="16">
+        <v>18.0</v>
+      </c>
+      <c r="B96" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C96" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D96" t="n" s="20">
-        <v>3700.0</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D96" s="16"/>
     </row>
     <row r="97">
       <c r="A97" s="27"/>
       <c r="C97" t="s" s="19">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D97" t="n" s="20">
-        <v>2700.0</v>
+        <v>3300.0</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="27"/>
       <c r="C98" t="s" s="19">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D98" t="n" s="20">
-        <v>1600.0</v>
+        <v>2700.0</v>
       </c>
     </row>
     <row r="99">
@@ -1618,29 +1586,29 @@
     </row>
     <row r="100">
       <c r="A100" t="n" s="16">
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
       <c r="B100" t="n" s="17">
         <v>46026.0</v>
       </c>
       <c r="C100" t="s" s="19">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D100" s="16"/>
     </row>
     <row r="101">
       <c r="A101" s="27"/>
       <c r="C101" t="s" s="19">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D101" t="n" s="20">
-        <v>4100.0</v>
+        <v>3700.0</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="27"/>
       <c r="C102" t="s" s="19">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D102" t="n" s="20">
         <v>1800.0</v>
@@ -1649,7 +1617,7 @@
     <row r="103">
       <c r="A103" s="27"/>
       <c r="C103" t="s" s="19">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D103" t="n" s="20">
         <v>1200.0</v>
@@ -1661,29 +1629,29 @@
     </row>
     <row r="105">
       <c r="A105" t="n" s="16">
-        <v>19.0</v>
+        <v>20.0</v>
       </c>
       <c r="B105" t="n" s="17">
         <v>46026.0</v>
       </c>
       <c r="C105" t="s" s="19">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D105" s="16"/>
     </row>
     <row r="106">
       <c r="A106" s="27"/>
       <c r="C106" t="s" s="19">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D106" t="n" s="20">
-        <v>2500.0</v>
+        <v>4100.0</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="27"/>
       <c r="C107" t="s" s="19">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D107" t="n" s="20">
         <v>2100.0</v>
@@ -1691,45 +1659,45 @@
     </row>
     <row r="108">
       <c r="A108" s="27"/>
-      <c r="D108" s="31"/>
+      <c r="C108" t="s" s="19">
+        <v>15</v>
+      </c>
+      <c r="D108" t="n" s="20">
+        <v>1600.0</v>
+      </c>
     </row>
     <row r="109">
-      <c r="A109" t="n" s="16">
-        <v>20.0</v>
-      </c>
-      <c r="B109" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C109" t="s" s="19">
-        <v>42</v>
-      </c>
-      <c r="D109" s="16"/>
+      <c r="A109" s="27"/>
+      <c r="D109" s="31"/>
     </row>
     <row r="110">
-      <c r="A110" s="27"/>
+      <c r="A110" t="n" s="16">
+        <v>21.0</v>
+      </c>
+      <c r="B110" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C110" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D110" t="n" s="20">
-        <v>2900.0</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D110" s="16"/>
     </row>
     <row r="111">
       <c r="A111" s="27"/>
       <c r="C111" t="s" s="19">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D111" t="n" s="20">
-        <v>2400.0</v>
+        <v>2500.0</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="27"/>
       <c r="C112" t="s" s="19">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D112" t="n" s="20">
-        <v>1600.0</v>
+        <v>2400.0</v>
       </c>
     </row>
     <row r="113">
@@ -1738,176 +1706,176 @@
         <v>18</v>
       </c>
       <c r="D113" t="n" s="20">
-        <v>1200.0</v>
+        <v>1400.0</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="27"/>
-      <c r="D114" s="31"/>
+      <c r="C114" t="s" s="19">
+        <v>13</v>
+      </c>
+      <c r="D114" t="n" s="20">
+        <v>1200.0</v>
+      </c>
     </row>
     <row r="115">
-      <c r="A115" t="n" s="16">
-        <v>21.0</v>
-      </c>
-      <c r="B115" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C115" t="s" s="19">
-        <v>43</v>
-      </c>
-      <c r="D115" s="16"/>
+      <c r="A115" s="27"/>
+      <c r="D115" s="31"/>
     </row>
     <row r="116">
-      <c r="A116" s="27"/>
+      <c r="A116" t="n" s="16">
+        <v>22.0</v>
+      </c>
+      <c r="B116" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C116" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D116" t="n" s="20">
-        <v>3300.0</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D116" s="16"/>
     </row>
     <row r="117">
       <c r="A117" s="27"/>
       <c r="C117" t="s" s="19">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D117" t="n" s="20">
-        <v>2700.0</v>
+        <v>2900.0</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="27"/>
-      <c r="D118" s="31"/>
+      <c r="C118" t="s" s="19">
+        <v>12</v>
+      </c>
+      <c r="D118" t="n" s="20">
+        <v>2700.0</v>
+      </c>
     </row>
     <row r="119">
-      <c r="A119" t="n" s="16">
-        <v>22.0</v>
-      </c>
-      <c r="B119" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C119" t="s" s="19">
-        <v>44</v>
-      </c>
-      <c r="D119" s="16"/>
+      <c r="A119" s="27"/>
+      <c r="D119" s="31"/>
     </row>
     <row r="120">
-      <c r="A120" s="27"/>
+      <c r="A120" t="n" s="16">
+        <v>23.0</v>
+      </c>
+      <c r="B120" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C120" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D120" t="n" s="20">
-        <v>3700.0</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D120" s="16"/>
     </row>
     <row r="121">
       <c r="A121" s="27"/>
       <c r="C121" t="s" s="19">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D121" t="n" s="20">
-        <v>1800.0</v>
+        <v>3300.0</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="27"/>
       <c r="C122" t="s" s="19">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D122" t="n" s="20">
-        <v>1200.0</v>
+        <v>1800.0</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="27"/>
-      <c r="D123" s="31"/>
+      <c r="C123" t="s" s="19">
+        <v>15</v>
+      </c>
+      <c r="D123" t="n" s="20">
+        <v>1600.0</v>
+      </c>
     </row>
     <row r="124">
-      <c r="A124" t="n" s="16">
-        <v>23.0</v>
-      </c>
-      <c r="B124" t="n" s="17">
-        <v>46026.0</v>
-      </c>
+      <c r="A124" s="27"/>
       <c r="C124" t="s" s="19">
-        <v>45</v>
-      </c>
-      <c r="D124" s="16"/>
+        <v>13</v>
+      </c>
+      <c r="D124" t="n" s="20">
+        <v>1200.0</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="27"/>
-      <c r="C125" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D125" t="n" s="20">
-        <v>4100.0</v>
-      </c>
+      <c r="D125" s="31"/>
     </row>
     <row r="126">
-      <c r="A126" s="27"/>
+      <c r="A126" t="n" s="16">
+        <v>24.0</v>
+      </c>
+      <c r="B126" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C126" t="s" s="19">
-        <v>25</v>
-      </c>
-      <c r="D126" t="n" s="20">
-        <v>2100.0</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D126" s="16"/>
     </row>
     <row r="127">
       <c r="A127" s="27"/>
       <c r="C127" t="s" s="19">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D127" t="n" s="20">
-        <v>1600.0</v>
+        <v>3700.0</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="27"/>
-      <c r="D128" s="31"/>
+      <c r="C128" t="s" s="19">
+        <v>12</v>
+      </c>
+      <c r="D128" t="n" s="20">
+        <v>2100.0</v>
+      </c>
     </row>
     <row r="129">
-      <c r="A129" t="n" s="16">
-        <v>24.0</v>
-      </c>
-      <c r="B129" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C129" t="s" s="19">
-        <v>46</v>
-      </c>
-      <c r="D129" s="16"/>
+      <c r="A129" s="27"/>
+      <c r="D129" s="31"/>
     </row>
     <row r="130">
-      <c r="A130" s="27"/>
+      <c r="A130" t="n" s="16">
+        <v>25.0</v>
+      </c>
+      <c r="B130" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C130" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D130" t="n" s="20">
-        <v>2500.0</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D130" s="16"/>
     </row>
     <row r="131">
       <c r="A131" s="27"/>
       <c r="C131" t="s" s="19">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D131" t="n" s="20">
-        <v>2400.0</v>
+        <v>4100.0</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="27"/>
       <c r="C132" t="s" s="19">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D132" t="n" s="20">
-        <v>1400.0</v>
+        <v>2400.0</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="27"/>
       <c r="C133" t="s" s="19">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D133" t="n" s="20">
         <v>1200.0</v>
@@ -1919,29 +1887,29 @@
     </row>
     <row r="135">
       <c r="A135" t="n" s="16">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="B135" t="n" s="17">
         <v>46026.0</v>
       </c>
       <c r="C135" t="s" s="19">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D135" s="16"/>
     </row>
     <row r="136">
       <c r="A136" s="27"/>
       <c r="C136" t="s" s="19">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D136" t="n" s="20">
-        <v>2900.0</v>
+        <v>2500.0</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="27"/>
       <c r="C137" t="s" s="19">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D137" t="n" s="20">
         <v>2700.0</v>
@@ -1949,51 +1917,51 @@
     </row>
     <row r="138">
       <c r="A138" s="27"/>
-      <c r="D138" s="31"/>
+      <c r="C138" t="s" s="19">
+        <v>15</v>
+      </c>
+      <c r="D138" t="n" s="20">
+        <v>1600.0</v>
+      </c>
     </row>
     <row r="139">
-      <c r="A139" t="n" s="16">
-        <v>26.0</v>
-      </c>
-      <c r="B139" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C139" t="s" s="19">
-        <v>48</v>
-      </c>
-      <c r="D139" s="16"/>
+      <c r="A139" s="27"/>
+      <c r="D139" s="31"/>
     </row>
     <row r="140">
-      <c r="A140" s="27"/>
+      <c r="A140" t="n" s="16">
+        <v>27.0</v>
+      </c>
+      <c r="B140" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C140" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D140" t="n" s="20">
-        <v>3300.0</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D140" s="16"/>
     </row>
     <row r="141">
       <c r="A141" s="27"/>
       <c r="C141" t="s" s="19">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D141" t="n" s="20">
-        <v>1800.0</v>
+        <v>2900.0</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="27"/>
       <c r="C142" t="s" s="19">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D142" t="n" s="20">
-        <v>1600.0</v>
+        <v>1800.0</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="27"/>
       <c r="C143" t="s" s="19">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D143" t="n" s="20">
         <v>1200.0</v>
@@ -2005,29 +1973,29 @@
     </row>
     <row r="145">
       <c r="A145" t="n" s="16">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
       <c r="B145" t="n" s="17">
         <v>46026.0</v>
       </c>
       <c r="C145" t="s" s="19">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D145" s="16"/>
     </row>
     <row r="146">
       <c r="A146" s="27"/>
       <c r="C146" t="s" s="19">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D146" t="n" s="20">
-        <v>3700.0</v>
+        <v>3300.0</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="27"/>
       <c r="C147" t="s" s="19">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D147" t="n" s="20">
         <v>2100.0</v>
@@ -2039,29 +2007,29 @@
     </row>
     <row r="149">
       <c r="A149" t="n" s="16">
-        <v>28.0</v>
+        <v>29.0</v>
       </c>
       <c r="B149" t="n" s="17">
         <v>46026.0</v>
       </c>
       <c r="C149" t="s" s="19">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D149" s="16"/>
     </row>
     <row r="150">
       <c r="A150" s="27"/>
       <c r="C150" t="s" s="19">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D150" t="n" s="20">
-        <v>4100.0</v>
+        <v>3700.0</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="27"/>
       <c r="C151" t="s" s="19">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D151" t="n" s="20">
         <v>2400.0</v>
@@ -2070,53 +2038,53 @@
     <row r="152">
       <c r="A152" s="27"/>
       <c r="C152" t="s" s="19">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D152" t="n" s="20">
-        <v>1200.0</v>
+        <v>1600.0</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="27"/>
-      <c r="D153" s="31"/>
+      <c r="C153" t="s" s="19">
+        <v>13</v>
+      </c>
+      <c r="D153" t="n" s="20">
+        <v>1200.0</v>
+      </c>
     </row>
     <row r="154">
-      <c r="A154" t="n" s="16">
-        <v>29.0</v>
-      </c>
-      <c r="B154" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C154" t="s" s="19">
-        <v>51</v>
-      </c>
-      <c r="D154" s="16"/>
+      <c r="A154" s="27"/>
+      <c r="D154" s="31"/>
     </row>
     <row r="155">
-      <c r="A155" s="27"/>
+      <c r="A155" t="n" s="16">
+        <v>30.0</v>
+      </c>
+      <c r="B155" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C155" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D155" t="n" s="20">
-        <v>2500.0</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D155" s="16"/>
     </row>
     <row r="156">
       <c r="A156" s="27"/>
       <c r="C156" t="s" s="19">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D156" t="n" s="20">
-        <v>2700.0</v>
+        <v>4100.0</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="27"/>
       <c r="C157" t="s" s="19">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D157" t="n" s="20">
-        <v>1600.0</v>
+        <v>2700.0</v>
       </c>
     </row>
     <row r="158">
@@ -2125,29 +2093,29 @@
     </row>
     <row r="159">
       <c r="A159" t="n" s="16">
-        <v>30.0</v>
+        <v>31.0</v>
       </c>
       <c r="B159" t="n" s="17">
         <v>46026.0</v>
       </c>
       <c r="C159" t="s" s="19">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D159" s="16"/>
     </row>
     <row r="160">
       <c r="A160" s="27"/>
       <c r="C160" t="s" s="19">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D160" t="n" s="20">
-        <v>2900.0</v>
+        <v>2500.0</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="27"/>
       <c r="C161" t="s" s="19">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D161" t="n" s="20">
         <v>1800.0</v>
@@ -2159,394 +2127,394 @@
         <v>18</v>
       </c>
       <c r="D162" t="n" s="20">
-        <v>1200.0</v>
+        <v>1400.0</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="27"/>
-      <c r="D163" s="31"/>
+      <c r="C163" t="s" s="19">
+        <v>13</v>
+      </c>
+      <c r="D163" t="n" s="20">
+        <v>1200.0</v>
+      </c>
     </row>
     <row r="164">
-      <c r="A164" t="n" s="16">
-        <v>31.0</v>
-      </c>
-      <c r="B164" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C164" t="s" s="19">
-        <v>53</v>
-      </c>
-      <c r="D164" s="16"/>
+      <c r="A164" s="27"/>
+      <c r="D164" s="31"/>
     </row>
     <row r="165">
-      <c r="A165" s="27"/>
+      <c r="A165" t="n" s="16">
+        <v>32.0</v>
+      </c>
+      <c r="B165" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C165" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D165" t="n" s="20">
-        <v>3300.0</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D165" s="16"/>
     </row>
     <row r="166">
       <c r="A166" s="27"/>
       <c r="C166" t="s" s="19">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D166" t="n" s="20">
-        <v>2100.0</v>
+        <v>2900.0</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="27"/>
-      <c r="D167" s="31"/>
+      <c r="C167" t="s" s="19">
+        <v>12</v>
+      </c>
+      <c r="D167" t="n" s="20">
+        <v>2100.0</v>
+      </c>
     </row>
     <row r="168">
-      <c r="A168" t="n" s="16">
-        <v>32.0</v>
-      </c>
-      <c r="B168" t="n" s="17">
-        <v>46026.0</v>
-      </c>
+      <c r="A168" s="27"/>
       <c r="C168" t="s" s="19">
-        <v>54</v>
-      </c>
-      <c r="D168" s="16"/>
+        <v>15</v>
+      </c>
+      <c r="D168" t="n" s="20">
+        <v>1600.0</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="27"/>
-      <c r="C169" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D169" t="n" s="20">
-        <v>3700.0</v>
-      </c>
+      <c r="D169" s="31"/>
     </row>
     <row r="170">
-      <c r="A170" s="27"/>
+      <c r="A170" t="n" s="16">
+        <v>33.0</v>
+      </c>
+      <c r="B170" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C170" t="s" s="19">
-        <v>25</v>
-      </c>
-      <c r="D170" t="n" s="20">
-        <v>2400.0</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D170" s="16"/>
     </row>
     <row r="171">
       <c r="A171" s="27"/>
       <c r="C171" t="s" s="19">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D171" t="n" s="20">
-        <v>1600.0</v>
+        <v>3300.0</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="27"/>
       <c r="C172" t="s" s="19">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D172" t="n" s="20">
-        <v>1200.0</v>
+        <v>2400.0</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="27"/>
-      <c r="D173" s="31"/>
+      <c r="C173" t="s" s="19">
+        <v>13</v>
+      </c>
+      <c r="D173" t="n" s="20">
+        <v>1200.0</v>
+      </c>
     </row>
     <row r="174">
-      <c r="A174" t="n" s="16">
-        <v>33.0</v>
-      </c>
-      <c r="B174" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C174" t="s" s="19">
-        <v>55</v>
-      </c>
-      <c r="D174" s="16"/>
+      <c r="A174" s="27"/>
+      <c r="D174" s="31"/>
     </row>
     <row r="175">
-      <c r="A175" s="27"/>
+      <c r="A175" t="n" s="16">
+        <v>34.0</v>
+      </c>
+      <c r="B175" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C175" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D175" t="n" s="20">
-        <v>4100.0</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="D175" s="16"/>
     </row>
     <row r="176">
       <c r="A176" s="27"/>
       <c r="C176" t="s" s="19">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D176" t="n" s="20">
-        <v>2700.0</v>
+        <v>3700.0</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="27"/>
-      <c r="D177" s="31"/>
+      <c r="C177" t="s" s="19">
+        <v>12</v>
+      </c>
+      <c r="D177" t="n" s="20">
+        <v>2700.0</v>
+      </c>
     </row>
     <row r="178">
-      <c r="A178" t="n" s="16">
-        <v>34.0</v>
-      </c>
-      <c r="B178" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C178" t="s" s="19">
-        <v>56</v>
-      </c>
-      <c r="D178" s="16"/>
+      <c r="A178" s="27"/>
+      <c r="D178" s="31"/>
     </row>
     <row r="179">
-      <c r="A179" s="27"/>
+      <c r="A179" t="n" s="16">
+        <v>35.0</v>
+      </c>
+      <c r="B179" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C179" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D179" t="n" s="20">
-        <v>2500.0</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D179" s="16"/>
     </row>
     <row r="180">
       <c r="A180" s="27"/>
       <c r="C180" t="s" s="19">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D180" t="n" s="20">
-        <v>1800.0</v>
+        <v>4100.0</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="27"/>
       <c r="C181" t="s" s="19">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D181" t="n" s="20">
-        <v>1400.0</v>
+        <v>1800.0</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="27"/>
       <c r="C182" t="s" s="19">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D182" t="n" s="20">
-        <v>1200.0</v>
+        <v>1600.0</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="27"/>
-      <c r="D183" s="31"/>
+      <c r="C183" t="s" s="19">
+        <v>13</v>
+      </c>
+      <c r="D183" t="n" s="20">
+        <v>1200.0</v>
+      </c>
     </row>
     <row r="184">
-      <c r="A184" t="n" s="16">
-        <v>35.0</v>
-      </c>
-      <c r="B184" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C184" t="s" s="19">
-        <v>57</v>
-      </c>
-      <c r="D184" s="16"/>
+      <c r="A184" s="27"/>
+      <c r="D184" s="31"/>
     </row>
     <row r="185">
-      <c r="A185" s="27"/>
+      <c r="A185" t="n" s="16">
+        <v>36.0</v>
+      </c>
+      <c r="B185" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C185" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D185" t="n" s="20">
-        <v>2900.0</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="D185" s="16"/>
     </row>
     <row r="186">
       <c r="A186" s="27"/>
       <c r="C186" t="s" s="19">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D186" t="n" s="20">
-        <v>2100.0</v>
+        <v>2500.0</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="27"/>
       <c r="C187" t="s" s="19">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D187" t="n" s="20">
-        <v>1600.0</v>
+        <v>2100.0</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="27"/>
-      <c r="D188" s="31"/>
+      <c r="C188" t="s" s="19">
+        <v>18</v>
+      </c>
+      <c r="D188" t="n" s="20">
+        <v>1400.0</v>
+      </c>
     </row>
     <row r="189">
-      <c r="A189" t="n" s="16">
-        <v>36.0</v>
-      </c>
-      <c r="B189" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C189" t="s" s="19">
-        <v>58</v>
-      </c>
-      <c r="D189" s="16"/>
+      <c r="A189" s="27"/>
+      <c r="D189" s="31"/>
     </row>
     <row r="190">
-      <c r="A190" s="27"/>
+      <c r="A190" t="n" s="16">
+        <v>37.0</v>
+      </c>
+      <c r="B190" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C190" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D190" t="n" s="20">
-        <v>3300.0</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D190" s="16"/>
     </row>
     <row r="191">
       <c r="A191" s="27"/>
       <c r="C191" t="s" s="19">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D191" t="n" s="20">
-        <v>2400.0</v>
+        <v>2900.0</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="27"/>
       <c r="C192" t="s" s="19">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D192" t="n" s="20">
-        <v>1200.0</v>
+        <v>2400.0</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="27"/>
-      <c r="D193" s="31"/>
+      <c r="C193" t="s" s="19">
+        <v>13</v>
+      </c>
+      <c r="D193" t="n" s="20">
+        <v>1200.0</v>
+      </c>
     </row>
     <row r="194">
-      <c r="A194" t="n" s="16">
-        <v>37.0</v>
-      </c>
-      <c r="B194" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C194" t="s" s="19">
-        <v>59</v>
-      </c>
-      <c r="D194" s="16"/>
+      <c r="A194" s="27"/>
+      <c r="D194" s="31"/>
     </row>
     <row r="195">
-      <c r="A195" s="27"/>
+      <c r="A195" t="n" s="16">
+        <v>38.0</v>
+      </c>
+      <c r="B195" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C195" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D195" t="n" s="20">
-        <v>3700.0</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="D195" s="16"/>
     </row>
     <row r="196">
       <c r="A196" s="27"/>
       <c r="C196" t="s" s="19">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D196" t="n" s="20">
-        <v>2700.0</v>
+        <v>3300.0</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="27"/>
-      <c r="D197" s="31"/>
+      <c r="C197" t="s" s="19">
+        <v>12</v>
+      </c>
+      <c r="D197" t="n" s="20">
+        <v>2700.0</v>
+      </c>
     </row>
     <row r="198">
-      <c r="A198" t="n" s="16">
-        <v>38.0</v>
-      </c>
-      <c r="B198" t="n" s="17">
-        <v>46026.0</v>
-      </c>
+      <c r="A198" s="27"/>
       <c r="C198" t="s" s="19">
-        <v>60</v>
-      </c>
-      <c r="D198" s="16"/>
+        <v>15</v>
+      </c>
+      <c r="D198" t="n" s="20">
+        <v>1600.0</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" s="27"/>
-      <c r="C199" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D199" t="n" s="20">
-        <v>4100.0</v>
-      </c>
+      <c r="D199" s="31"/>
     </row>
     <row r="200">
-      <c r="A200" s="27"/>
+      <c r="A200" t="n" s="16">
+        <v>39.0</v>
+      </c>
+      <c r="B200" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C200" t="s" s="19">
-        <v>25</v>
-      </c>
-      <c r="D200" t="n" s="20">
-        <v>1800.0</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D200" s="16"/>
     </row>
     <row r="201">
       <c r="A201" s="27"/>
       <c r="C201" t="s" s="19">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D201" t="n" s="20">
-        <v>1600.0</v>
+        <v>3700.0</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="27"/>
       <c r="C202" t="s" s="19">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D202" t="n" s="20">
-        <v>1200.0</v>
+        <v>1800.0</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="27"/>
-      <c r="D203" s="31"/>
+      <c r="C203" t="s" s="19">
+        <v>13</v>
+      </c>
+      <c r="D203" t="n" s="20">
+        <v>1200.0</v>
+      </c>
     </row>
     <row r="204">
-      <c r="A204" t="n" s="16">
-        <v>39.0</v>
-      </c>
-      <c r="B204" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C204" t="s" s="19">
-        <v>61</v>
-      </c>
-      <c r="D204" s="16"/>
+      <c r="A204" s="27"/>
+      <c r="D204" s="31"/>
     </row>
     <row r="205">
-      <c r="A205" s="27"/>
+      <c r="A205" t="n" s="16">
+        <v>40.0</v>
+      </c>
+      <c r="B205" t="n" s="17">
+        <v>46026.0</v>
+      </c>
       <c r="C205" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D205" t="n" s="20">
-        <v>2500.0</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D205" s="16"/>
     </row>
     <row r="206">
       <c r="A206" s="27"/>
       <c r="C206" t="s" s="19">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="D206" t="n" s="20">
-        <v>2100.0</v>
+        <v>4100.0</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="27"/>
       <c r="C207" t="s" s="19">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D207" t="n" s="20">
-        <v>1400.0</v>
+        <v>2100.0</v>
       </c>
     </row>
     <row r="208">
@@ -2554,176 +2522,13 @@
       <c r="D208" s="31"/>
     </row>
     <row r="209">
-      <c r="A209" t="n" s="16">
-        <v>40.0</v>
-      </c>
-      <c r="B209" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C209" t="s" s="19">
-        <v>62</v>
-      </c>
-      <c r="D209" s="16"/>
-    </row>
-    <row r="210">
-      <c r="A210" s="27"/>
-      <c r="C210" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D210" t="n" s="20">
-        <v>2900.0</v>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" s="27"/>
-      <c r="C211" t="s" s="19">
-        <v>25</v>
-      </c>
-      <c r="D211" t="n" s="20">
-        <v>2400.0</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" s="27"/>
-      <c r="C212" t="s" s="19">
-        <v>18</v>
-      </c>
-      <c r="D212" t="n" s="20">
-        <v>1200.0</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" s="27"/>
-      <c r="D213" s="31"/>
-    </row>
-    <row r="214">
-      <c r="A214" t="n" s="16">
-        <v>41.0</v>
-      </c>
-      <c r="B214" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C214" t="s" s="19">
-        <v>63</v>
-      </c>
-      <c r="D214" s="16"/>
-    </row>
-    <row r="215">
-      <c r="A215" s="27"/>
-      <c r="C215" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D215" t="n" s="20">
-        <v>3300.0</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" s="27"/>
-      <c r="C216" t="s" s="19">
-        <v>25</v>
-      </c>
-      <c r="D216" t="n" s="20">
-        <v>2700.0</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" s="27"/>
-      <c r="C217" t="s" s="19">
-        <v>17</v>
-      </c>
-      <c r="D217" t="n" s="20">
-        <v>1600.0</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" s="27"/>
-      <c r="D218" s="31"/>
-    </row>
-    <row r="219">
-      <c r="A219" t="n" s="16">
-        <v>42.0</v>
-      </c>
-      <c r="B219" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C219" t="s" s="19">
-        <v>64</v>
-      </c>
-      <c r="D219" s="16"/>
-    </row>
-    <row r="220">
-      <c r="A220" s="27"/>
-      <c r="C220" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D220" t="n" s="20">
-        <v>3700.0</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" s="27"/>
-      <c r="C221" t="s" s="19">
-        <v>25</v>
-      </c>
-      <c r="D221" t="n" s="20">
-        <v>1800.0</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" s="27"/>
-      <c r="C222" t="s" s="19">
-        <v>18</v>
-      </c>
-      <c r="D222" t="n" s="20">
-        <v>1200.0</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" s="27"/>
-      <c r="D223" s="31"/>
-    </row>
-    <row r="224">
-      <c r="A224" t="n" s="16">
-        <v>43.0</v>
-      </c>
-      <c r="B224" t="n" s="17">
-        <v>46026.0</v>
-      </c>
-      <c r="C224" t="s" s="19">
-        <v>65</v>
-      </c>
-      <c r="D224" s="16"/>
-    </row>
-    <row r="225">
-      <c r="A225" s="27"/>
-      <c r="C225" t="s" s="19">
-        <v>24</v>
-      </c>
-      <c r="D225" t="n" s="20">
-        <v>4100.0</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" s="27"/>
-      <c r="C226" t="s" s="19">
-        <v>25</v>
-      </c>
-      <c r="D226" t="n" s="20">
-        <v>2100.0</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" s="27"/>
-      <c r="D227" s="31"/>
-    </row>
-    <row r="228">
-      <c r="A228" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B228" s="22"/>
-      <c r="C228" s="22"/>
-      <c r="D228" t="n" s="21">
-        <v>288600.0</v>
+      <c r="A209" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B209" s="22"/>
+      <c r="C209" s="22"/>
+      <c r="D209" t="n" s="21">
+        <v>275200.0</v>
       </c>
     </row>
   </sheetData>
@@ -2734,9 +2539,10 @@
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A228:C228"/>
+    <mergeCell ref="A209:C209"/>
   </mergeCells>
+  <printOptions horizontalCentered="true"/>
   <pageMargins bottom="0.5" footer="0.3" header="0.3" left="0.3" right="0.7" top="0.5"/>
-  <pageSetup paperSize="9" fitToWidth="1"/>
+  <pageSetup paperSize="9" fitToWidth="1" fitToHeight="0" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>